<commit_message>
add new mdpi doc
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\Documents\PhD stuff\Literature Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CED20A-D7F9-497B-B39D-B55AD33D9BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AC743A-FD94-4BB9-9440-D835520CAE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E9D36B1F-B9B3-4197-B5F4-3831E3A01BC7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="264">
   <si>
     <t>Reference</t>
   </si>
@@ -939,6 +939,24 @@
   </si>
   <si>
     <t>KnE</t>
+  </si>
+  <si>
+    <t>Bourahmoune et al. 2022</t>
+  </si>
+  <si>
+    <t>9 E-Textile Pressure Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile App &amp; Haptic Feedback </t>
+  </si>
+  <si>
+    <t>Upright, Slouching Forward, Extreme Slouching Forward, Leaning Back, Extreme Leaning Back, Left Shoulder Slouch, Right Shoulder Slouch, Left Side Slouch, Right Side Slouch, Left Lumbar Slouch, Right Lumbar Slouch, Rounded Shoulders, Forward Head Posture, Slight Correction Needed, and No User</t>
+  </si>
+  <si>
+    <t>Placed on the seat's back rest</t>
+  </si>
+  <si>
+    <t>decision trees-classification and regression trees (DT-CART), Random Forest (RF), k-nearest neighbors (k-NN), linear regression (LR), linear discriminant analysis (LDA), naive Bayes (NB), and neural network-multilayer perceptron (MLP)</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1120,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1139,6 +1157,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="8" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1303,9 +1324,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sitting Posture System'!$B$2:$B$29</c:f>
+              <c:f>'Sitting Posture System'!$B$2:$B$34</c:f>
               <c:strCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>Pereira and Plácido Da Silva, 2023</c:v>
                 </c:pt>
@@ -1389,16 +1410,31 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>R. et al, 2023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Fu and MacLeod, 2014</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>AbuTerkia et al, 2022</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Xu et al, 2013</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>La Mura et al, 2023</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Haeyoon Cho et al</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sitting Posture System'!$E$2:$E$29</c:f>
+              <c:f>'Sitting Posture System'!$E$2:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -1479,6 +1515,21 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3237,15 +3288,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>126771</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>149831</xdr:rowOff>
+      <xdr:colOff>141654</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>45651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>138111</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>161171</xdr:rowOff>
+      <xdr:colOff>152994</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>56991</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3608,8 +3659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5AB66E-634F-4264-B1B7-3EC9A3CB3421}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+    <sheetView tabSelected="1" topLeftCell="E15" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5047,10 +5098,48 @@
         <v>118</v>
       </c>
     </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="I35">
+        <v>18</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="L35" t="s">
+        <v>61</v>
+      </c>
+      <c r="N35" t="s">
+        <v>263</v>
+      </c>
+    </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E44">
-        <f>AVERAGE(E2:E34)</f>
-        <v>7.290322580645161</v>
+        <f>AVERAGE(E2:E35)</f>
+        <v>7.53125</v>
       </c>
       <c r="G44" t="s">
         <v>12</v>
@@ -5069,7 +5158,7 @@
         <v>97</v>
       </c>
       <c r="E45">
-        <f>MAX(E2:E34)</f>
+        <f>MAX(E2:E35)</f>
         <v>15</v>
       </c>
       <c r="H45" s="1">
@@ -5086,7 +5175,7 @@
         <v>98</v>
       </c>
       <c r="E46">
-        <f>MIN(E2:E34)</f>
+        <f>MIN(E2:E35)</f>
         <v>3</v>
       </c>
       <c r="H46" s="1">

</xml_diff>